<commit_message>
new model for gen scheme
</commit_message>
<xml_diff>
--- a/Arch.xlsx
+++ b/Arch.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="10">
   <si>
     <t xml:space="preserve">h</t>
   </si>
@@ -151,19 +151,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:AA41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="10" min="1" style="1" width="9.99595141700405"/>
+    <col collapsed="false" hidden="false" max="10" min="1" style="1" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="24" min="12" style="1" width="9.99595141700405"/>
+    <col collapsed="false" hidden="false" max="24" min="12" style="1" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="9.99595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="10.0688259109312"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -277,21 +277,21 @@
         <v>30</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">ROUNDDOWN((B3+2*D3-(C3-1)-1)/E3+1,0)</f>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="n">
         <f aca="false">F5</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>3</v>
@@ -307,7 +307,7 @@
       </c>
       <c r="M3" s="1" t="n">
         <f aca="false">(H3-1)*L3-2*J3+I3+K3</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P3" s="1" t="n">
         <v>90</v>
@@ -349,7 +349,7 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="n">
         <f aca="false">F3</f>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>3</v>
@@ -362,11 +362,11 @@
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">ROUNDDOWN((B4+2*D4-(C4-1)-1)/E4+1,0)</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="n">
         <f aca="false">M3</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>3</v>
@@ -382,7 +382,7 @@
       </c>
       <c r="M4" s="1" t="n">
         <f aca="false">(H4-1)*L4-2*J4+I4+K4</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="P4" s="1" t="n">
         <f aca="false">T3</f>
@@ -425,7 +425,7 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="n">
         <f aca="false">F4</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>3</v>
@@ -438,11 +438,11 @@
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">ROUNDDOWN((B5+2*D5-(C5-1)-1)/E5+1,0)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H5" s="1" t="n">
         <f aca="false">M4</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>3</v>
@@ -458,7 +458,7 @@
       </c>
       <c r="M5" s="1" t="n">
         <f aca="false">(H5-1)*L5-2*J5+I5+K5</f>
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="P5" s="1" t="n">
         <f aca="false">T4</f>
@@ -499,9 +499,14 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
       <c r="H6" s="1" t="n">
         <f aca="false">M5</f>
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>3</v>
@@ -517,8 +522,13 @@
       </c>
       <c r="M6" s="1" t="n">
         <f aca="false">(H6-1)*L6-2*J6+I6+K6</f>
-        <v>30</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
+      <c r="S6" s="0"/>
+      <c r="T6" s="0"/>
       <c r="V6" s="1" t="n">
         <f aca="false">AA5</f>
         <v>29</v>
@@ -540,7 +550,26 @@
         <v>30</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+    </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="I8" s="0"/>
       <c r="P8" s="0"/>
       <c r="Q8" s="0"/>
       <c r="R8" s="0"/>
@@ -548,6 +577,22 @@
       <c r="T8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="0"/>
       <c r="P9" s="0"/>
       <c r="Q9" s="0"/>
       <c r="R9" s="0"/>
@@ -555,6 +600,23 @@
       <c r="T9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B10+2*D10-(C10-1)-1)/E10+1,0)</f>
+        <v>43</v>
+      </c>
+      <c r="I10" s="0"/>
       <c r="P10" s="0"/>
       <c r="Q10" s="0"/>
       <c r="R10" s="0"/>
@@ -562,12 +624,59 @@
       <c r="T10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="n">
+        <f aca="false">F10</f>
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B11+2*D11-(C11-1)-1)/E11+1,0)</f>
+        <v>40</v>
+      </c>
+      <c r="I11" s="0"/>
       <c r="P11" s="0"/>
       <c r="Q11" s="0"/>
       <c r="R11" s="0"/>
       <c r="S11" s="0"/>
       <c r="T11" s="0"/>
     </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I12" s="0"/>
+      <c r="P12" s="0"/>
+      <c r="Q12" s="0"/>
+      <c r="R12" s="0"/>
+      <c r="S12" s="0"/>
+      <c r="T12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I13" s="0"/>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
+      <c r="T13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
+      <c r="S14" s="0"/>
+      <c r="T14" s="0"/>
+    </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -584,6 +693,7 @@
       <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="I15" s="0"/>
       <c r="P15" s="1" t="s">
         <v>4</v>
       </c>
@@ -605,18 +715,19 @@
         <v>30</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">ROUNDDOWN((B16+2*D16-(C16-1)-1)/E16+1,0)</f>
-        <v>30</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="I16" s="0"/>
       <c r="P16" s="1" t="n">
         <v>90</v>
       </c>
@@ -637,21 +748,22 @@
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="n">
         <f aca="false">F16</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">ROUNDDOWN((B17+2*D17-(C17-1)-1)/E17+1,0)</f>
-        <v>30</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="I17" s="0"/>
       <c r="P17" s="1" t="n">
         <f aca="false">T16</f>
         <v>42</v>
@@ -673,21 +785,22 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1" t="n">
         <f aca="false">F17</f>
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">ROUNDDOWN((B18+2*D18-(C18-1)-1)/E18+1,0)</f>
-        <v>30</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="I18" s="0"/>
       <c r="P18" s="1" t="n">
         <f aca="false">T17</f>
         <v>36</v>
@@ -706,13 +819,331 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1" t="n">
+        <f aca="false">F18</f>
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B19+2*D19-(C19-1)-1)/E19+1,0)</f>
+        <v>8</v>
+      </c>
+      <c r="I19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B23+2*D23-(C23-1)-1)/E23+1,0)</f>
+        <v>40</v>
+      </c>
+      <c r="I23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="n">
+        <f aca="false">F23</f>
+        <v>40</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B24+2*D24-(C24-1)-1)/E24+1,0)</f>
+        <v>40</v>
+      </c>
+      <c r="I24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="n">
+        <f aca="false">F24</f>
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B25+2*D25-(C25-1)-1)/E25+1,0)</f>
+        <v>40</v>
+      </c>
+      <c r="I25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="n">
+        <f aca="false">F25</f>
+        <v>40</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B26+2*D26-(C26-1)-1)/E26+1,0)</f>
+        <v>40</v>
+      </c>
+      <c r="I26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B31+2*D31-(C31-1)-1)/E31+1,0)</f>
+        <v>43</v>
+      </c>
+      <c r="I31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="n">
+        <f aca="false">F31</f>
+        <v>43</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B32+2*D32-(C32-1)-1)/E32+1,0)</f>
+        <v>38</v>
+      </c>
+      <c r="I32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="n">
+        <f aca="false">F32</f>
+        <v>38</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B33+2*D33-(C33-1)-1)/E33+1,0)</f>
+        <v>35</v>
+      </c>
+      <c r="I33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1" t="n">
+        <f aca="false">F33</f>
+        <v>35</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B34+2*D34-(C34-1)-1)/E34+1,0)</f>
+        <v>30</v>
+      </c>
       <c r="I34" s="1" t="n">
         <f aca="false">32*40*14</f>
         <v>17920</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B38+2*D38-(C38-1)-1)/E38+1,0)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="n">
+        <f aca="false">F38</f>
+        <v>30</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B39+2*D39-(C39-1)-1)/E39+1,0)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1" t="n">
+        <f aca="false">F39</f>
+        <v>30</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B40+2*D40-(C40-1)-1)/E40+1,0)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1" t="n">
+        <f aca="false">F40</f>
+        <v>30</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B41+2*D41-(C41-1)-1)/E41+1,0)</f>
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
changes for new resolution
</commit_message>
<xml_diff>
--- a/Arch.xlsx
+++ b/Arch.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="11">
   <si>
     <t xml:space="preserve">h</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">o_padding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame Gen</t>
   </si>
 </sst>
 </file>
@@ -151,19 +154,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA41"/>
+  <dimension ref="A1:AA58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="10" min="1" style="1" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="24" min="12" style="1" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="10.0688259109312"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="12" style="1" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="11.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="1" width="10.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,6 +652,11 @@
       <c r="T11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
       <c r="I12" s="0"/>
       <c r="P12" s="0"/>
       <c r="Q12" s="0"/>
@@ -657,6 +665,11 @@
       <c r="T12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
       <c r="I13" s="0"/>
       <c r="P13" s="0"/>
       <c r="Q13" s="0"/>
@@ -840,9 +853,19 @@
       <c r="I19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
       <c r="I21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -943,12 +966,27 @@
       <c r="I26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
       <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
       <c r="I28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
       <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1051,7 +1089,20 @@
         <v>17920</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+    </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
         <v>4</v>
@@ -1144,10 +1195,213 @@
         <v>30</v>
       </c>
     </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B48+2*D48-(C48-1)-1)/E48+1,0)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="1" t="n">
+        <f aca="false">F48</f>
+        <v>42</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B49+2*D49-(C49-1)-1)/E49+1,0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="1" t="n">
+        <f aca="false">F49</f>
+        <v>14</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B50+2*D50-(C50-1)-1)/E50+1,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="1" t="n">
+        <f aca="false">F50</f>
+        <v>7</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B51+2*D51-(C51-1)-1)/E51+1,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0"/>
+      <c r="C52" s="0"/>
+      <c r="D52" s="0"/>
+      <c r="E52" s="0"/>
+      <c r="F52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0"/>
+      <c r="C53" s="0"/>
+      <c r="D53" s="0"/>
+      <c r="E53" s="0"/>
+      <c r="F53" s="0"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E55" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B55+2*D55-(C55-1)-1)/E55+1,0)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1" t="n">
+        <f aca="false">F55</f>
+        <v>50</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B56+2*D56-(C56-1)-1)/E56+1,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="1" t="n">
+        <f aca="false">F56</f>
+        <v>25</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B57+2*D57-(C57-1)-1)/E57+1,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="1" t="n">
+        <f aca="false">F57</f>
+        <v>12</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <f aca="false">ROUNDDOWN((B58+2*D58-(C58-1)-1)/E58+1,0)</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
generating data on the fly
</commit_message>
<xml_diff>
--- a/Arch.xlsx
+++ b/Arch.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="11">
   <si>
     <t xml:space="preserve">h</t>
   </si>
@@ -156,8 +156,8 @@
   </sheetPr>
   <dimension ref="A1:AA58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K29" activeCellId="0" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -706,7 +706,21 @@
       <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="0"/>
+      <c r="H15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="P15" s="1" t="s">
         <v>4</v>
       </c>
@@ -740,7 +754,22 @@
         <f aca="false">ROUNDDOWN((B16+2*D16-(C16-1)-1)/E16+1,0)</f>
         <v>15</v>
       </c>
-      <c r="I16" s="0"/>
+      <c r="H16" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H16+2*J16-(I16-1)-1)/K16+1,0)</f>
+        <v>100</v>
+      </c>
       <c r="P16" s="1" t="n">
         <v>90</v>
       </c>
@@ -776,7 +805,23 @@
         <f aca="false">ROUNDDOWN((B17+2*D17-(C17-1)-1)/E17+1,0)</f>
         <v>8</v>
       </c>
-      <c r="I17" s="0"/>
+      <c r="H17" s="1" t="n">
+        <f aca="false">L16</f>
+        <v>100</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H17+2*J17-(I17-1)-1)/K17+1,0)</f>
+        <v>50</v>
+      </c>
       <c r="P17" s="1" t="n">
         <f aca="false">T16</f>
         <v>42</v>
@@ -813,7 +858,23 @@
         <f aca="false">ROUNDDOWN((B18+2*D18-(C18-1)-1)/E18+1,0)</f>
         <v>8</v>
       </c>
-      <c r="I18" s="0"/>
+      <c r="H18" s="1" t="n">
+        <f aca="false">L17</f>
+        <v>50</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L18" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H18+2*J18-(I18-1)-1)/K18+1,0)</f>
+        <v>25</v>
+      </c>
       <c r="P18" s="1" t="n">
         <f aca="false">T17</f>
         <v>36</v>
@@ -850,15 +911,47 @@
         <f aca="false">ROUNDDOWN((B19+2*D19-(C19-1)-1)/E19+1,0)</f>
         <v>8</v>
       </c>
-      <c r="I19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H19" s="1" t="n">
+        <f aca="false">L18</f>
+        <v>25</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L19" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H19+2*J19-(I19-1)-1)/K19+1,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0"/>
       <c r="C20" s="0"/>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
-      <c r="I20" s="0"/>
+      <c r="H20" s="1" t="n">
+        <f aca="false">L19</f>
+        <v>13</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H20+2*J20-(I20-1)-1)/K20+1,0)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0"/>
@@ -903,7 +996,21 @@
         <f aca="false">ROUNDDOWN((B23+2*D23-(C23-1)-1)/E23+1,0)</f>
         <v>40</v>
       </c>
-      <c r="I23" s="0"/>
+      <c r="H23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="n">
@@ -923,7 +1030,22 @@
         <f aca="false">ROUNDDOWN((B24+2*D24-(C24-1)-1)/E24+1,0)</f>
         <v>40</v>
       </c>
-      <c r="I24" s="0"/>
+      <c r="H24" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H24+2*J24-(I24-1)-1)/K24+1,0)</f>
+        <v>114</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="n">
@@ -943,7 +1065,23 @@
         <f aca="false">ROUNDDOWN((B25+2*D25-(C25-1)-1)/E25+1,0)</f>
         <v>40</v>
       </c>
-      <c r="I25" s="0"/>
+      <c r="H25" s="1" t="n">
+        <f aca="false">L24</f>
+        <v>114</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L25" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H25+2*J25-(I25-1)-1)/K25+1,0)</f>
+        <v>56</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="n">
@@ -963,23 +1101,71 @@
         <f aca="false">ROUNDDOWN((B26+2*D26-(C26-1)-1)/E26+1,0)</f>
         <v>40</v>
       </c>
-      <c r="I26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H26" s="1" t="n">
+        <f aca="false">L25</f>
+        <v>56</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L26" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H26+2*J26-(I26-1)-1)/K26+1,0)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0"/>
       <c r="C27" s="0"/>
       <c r="D27" s="0"/>
       <c r="E27" s="0"/>
       <c r="F27" s="0"/>
-      <c r="I27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H27" s="1" t="n">
+        <f aca="false">L26</f>
+        <v>27</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L27" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H27+2*J27-(I27-1)-1)/K27+1,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0"/>
       <c r="C28" s="0"/>
       <c r="D28" s="0"/>
       <c r="E28" s="0"/>
       <c r="F28" s="0"/>
-      <c r="I28" s="0"/>
+      <c r="H28" s="1" t="n">
+        <f aca="false">L27</f>
+        <v>13</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L28" s="1" t="n">
+        <f aca="false">ROUNDDOWN((H28+2*J28-(I28-1)-1)/K28+1,0)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0"/>

</xml_diff>